<commit_message>
Adding alteration missed during xfer
</commit_message>
<xml_diff>
--- a/RedTeam_CMM_V1.xlsx
+++ b/RedTeam_CMM_V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc0tch\Documents\CMM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc0tch\Documents\CMM\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7782C89-0B6A-49D8-92CD-8D5E267151AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{303D8E51-4FBA-4C09-BED9-9ED94E75F9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19245" yWindow="90" windowWidth="38310" windowHeight="20820" xr2:uid="{94D6FA02-3BD5-4F95-BA04-B61DC13561F1}"/>
+    <workbookView xWindow="57645" yWindow="90" windowWidth="19065" windowHeight="20820" xr2:uid="{94D6FA02-3BD5-4F95-BA04-B61DC13561F1}"/>
   </bookViews>
   <sheets>
     <sheet name="CMM" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>Resource Management</t>
   </si>
   <si>
-    <t>Accounts, licenses, and recurring expenses are reviewed quarterly for need or expiration</t>
-  </si>
-  <si>
     <t>Tracking methods provide alerts or other easily identifiable information to indicate actions needed in the next thirty days</t>
   </si>
   <si>
@@ -457,21 +454,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>roadmap of current and future work in a distributed tool; leadership is responsible for accountability</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Accounts and licenses are centrally tracked, understood, and reviewed as needed by the Red Team</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>; Red Team account passwords are secured</t>
     </r>
   </si>
   <si>
@@ -612,12 +594,6 @@
   </si>
   <si>
     <t>The Red Team leverages automated CI/CD actions to expedite delivery and maintain quality of products</t>
-  </si>
-  <si>
-    <t>Licenses and accounts are only tracked upon reminder of expiration or renewal needs; ownership is dispersed across multiple people</t>
-  </si>
-  <si>
-    <t>One person tracks accounts, payment methods, or licenses; knowledge not available to the entire Red Team</t>
   </si>
   <si>
     <t>The Red Team uses a single set of externally accessed, static infrastructure for operations; infrastructure is manually set up  per operation with inconsistent configuration; infrastructure accounts for minimal OPSEC considerations</t>
@@ -1267,6 +1243,18 @@
   </si>
   <si>
     <t>The Red Team regularly discusses opportunities and uniformly decides to stay the course or pivot; retrospectives consistently deliver process/operational improvements; the Red Team roadmap is considered during organizational planning</t>
+  </si>
+  <si>
+    <t>Resources like licenses, accounts, or domains are only tracked upon reminder of expiration or renewal needs; ownership is dispersed across multiple people</t>
+  </si>
+  <si>
+    <t>One person tracks resources; knowledge not available to the entire Red Team</t>
+  </si>
+  <si>
+    <t>Resources are centrally tracked, understood, and reviewed as needed by the Red Team; Red Team account passwords are secured</t>
+  </si>
+  <si>
+    <t>Recurring expenses or other resources are reviewed quarterly for need or expiration</t>
   </si>
 </sst>
 </file>
@@ -1938,11 +1926,11 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1962,19 +1950,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1991,22 +1979,22 @@
     <row r="3" spans="1:8" ht="105.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2018,16 +2006,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="G4" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2039,16 +2027,16 @@
         <v>9</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2057,19 +2045,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2078,19 +2066,19 @@
         <v>12</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>69</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>70</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -2103,10 +2091,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>15</v>
@@ -2121,7 +2109,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>18</v>
@@ -2145,42 +2133,42 @@
         <v>23</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="F11" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="22" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="25"/>
@@ -2192,69 +2180,69 @@
     <row r="13" spans="1:8" ht="75.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>30</v>
-      </c>
       <c r="F13" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F14" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="G15" s="23" t="s">
         <v>62</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
@@ -2266,148 +2254,148 @@
     <row r="17" spans="1:7" ht="135.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="120" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="G20" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>77</v>
-      </c>
       <c r="D21" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="F21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="22" t="s">
         <v>87</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="75" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="135" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>40</v>
-      </c>
       <c r="E23" s="22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="105" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2419,84 +2407,84 @@
         <v>4</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="22" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="105" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="22" t="s">
         <v>143</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="22" t="s">
         <v>148</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="32"/>
@@ -2508,85 +2496,85 @@
     <row r="29" spans="1:7" ht="116.45" customHeight="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="G29" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="116.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="22" t="s">
+      <c r="E30" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="F30" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="G30" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="D31" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="E31" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>53</v>
-      </c>
       <c r="G31" s="22" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
@@ -2619,52 +2607,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="387" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2959,17 +2947,17 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2618A23-7192-4C37-970C-F0C1DE1142D7}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cdd62f4f-0f76-406d-bafb-c0159c105e45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="01098293-a8f5-4a21-8849-ffdc1d6b180f"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="01098293-a8f5-4a21-8849-ffdc1d6b180f"/>
-    <ds:schemaRef ds:uri="cdd62f4f-0f76-406d-bafb-c0159c105e45"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added scores and averages
I added a column for the current score and notes. There is an average calculation for each of the 4 categories and all 27 items. I don't think this merits a version change but wanted to contribute the changes we made as we went through this.
</commit_message>
<xml_diff>
--- a/RedTeam_CMM_V1.xlsx
+++ b/RedTeam_CMM_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc0tch\Documents\CMM\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orchijo\Documents\GitHub\redteamcmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{303D8E51-4FBA-4C09-BED9-9ED94E75F9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC10C1B-BCEC-4371-9360-2512EC3F0C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57645" yWindow="90" windowWidth="19065" windowHeight="20820" xr2:uid="{94D6FA02-3BD5-4F95-BA04-B61DC13561F1}"/>
+    <workbookView xWindow="1515" yWindow="4650" windowWidth="27075" windowHeight="15000" xr2:uid="{94D6FA02-3BD5-4F95-BA04-B61DC13561F1}"/>
   </bookViews>
   <sheets>
     <sheet name="CMM" sheetId="1" r:id="rId1"/>
@@ -34,26 +34,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={9E706013-C820-4DF1-BF76-353CB642232D}</author>
-  </authors>
-  <commentList>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{9E706013-C820-4DF1-BF76-353CB642232D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Revisit this language. Is in contrast to operational planning which has this type of relationship at a lower level; also conflicts with lower levels within itself where conversations are happening but apparently not yielding this fruit</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Category</t>
   </si>
@@ -1255,6 +1237,15 @@
   </si>
   <si>
     <t>Recurring expenses or other resources are reviewed quarterly for need or expiration</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1583,13 +1574,236 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1920,17 +2134,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE54315D-271A-4534-BB7F-33D01A04C51C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE54315D-271A-4534-BB7F-33D01A04C51C}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1939,10 +2153,11 @@
     <col min="2" max="2" width="29.28515625" style="35" customWidth="1"/>
     <col min="3" max="7" width="34.5703125" style="22" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="22.85546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1961,11 +2176,17 @@
       <c r="F1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1974,9 +2195,14 @@
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" ht="105.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="19"/>
+      <c r="H2" s="45">
+        <f>AVERAGE(H3:H11)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" ht="125.25" customHeight="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="21" t="s">
         <v>55</v>
@@ -1996,8 +2222,12 @@
       <c r="G3" s="22" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="38">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="15" t="s">
         <v>6</v>
@@ -2017,8 +2247,11 @@
       <c r="G4" s="22" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="15" t="s">
         <v>8</v>
@@ -2038,8 +2271,12 @@
       <c r="G5" s="22" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="38">
+        <v>1</v>
+      </c>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="15" t="s">
         <v>10</v>
@@ -2059,8 +2296,11 @@
       <c r="G6" s="22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="120" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="15" t="s">
         <v>12</v>
@@ -2080,9 +2320,12 @@
       <c r="G7" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="38">
+        <v>1</v>
+      </c>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="15" t="s">
         <v>13</v>
@@ -2102,8 +2345,11 @@
       <c r="G8" s="22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="15" t="s">
         <v>17</v>
@@ -2123,8 +2369,12 @@
       <c r="G9" s="22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="38">
+        <v>1</v>
+      </c>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="15" t="s">
         <v>22</v>
@@ -2144,8 +2394,11 @@
       <c r="G10" s="22" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="21" t="s">
         <v>25</v>
@@ -2165,8 +2418,12 @@
       <c r="G11" s="22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="40">
+        <v>1</v>
+      </c>
+      <c r="I11" s="21"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -2175,9 +2432,14 @@
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" ht="75.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="25"/>
+      <c r="H12" s="44">
+        <f>AVERAGE(H13:H15)</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" ht="75.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="15" t="s">
         <v>28</v>
@@ -2197,8 +2459,12 @@
       <c r="G13" s="22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="40">
+        <v>1</v>
+      </c>
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="1:9" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="15" t="s">
         <v>30</v>
@@ -2218,8 +2484,11 @@
       <c r="G14" s="22" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="15" t="s">
         <v>31</v>
@@ -2239,8 +2508,12 @@
       <c r="G15" s="23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="40">
+        <v>1</v>
+      </c>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>32</v>
       </c>
@@ -2249,9 +2522,14 @@
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" ht="135.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="28"/>
+      <c r="H16" s="43">
+        <f>AVERAGE(H17:H27)</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="29"/>
+    </row>
+    <row r="17" spans="1:9" ht="135.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="15" t="s">
         <v>122</v>
@@ -2271,8 +2549,12 @@
       <c r="G17" s="22" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="120" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="40">
+        <v>1</v>
+      </c>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" ht="120" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="21" t="s">
         <v>63</v>
@@ -2292,8 +2574,11 @@
       <c r="G18" s="22" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="21" t="s">
         <v>64</v>
@@ -2313,8 +2598,12 @@
       <c r="G19" s="22" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="40">
+        <v>1</v>
+      </c>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="15" t="s">
         <v>74</v>
@@ -2334,8 +2623,11 @@
       <c r="G20" s="22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="15" t="s">
         <v>75</v>
@@ -2355,8 +2647,12 @@
       <c r="G21" s="22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="75" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="40">
+        <v>1</v>
+      </c>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" ht="75" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="15" t="s">
         <v>77</v>
@@ -2376,8 +2672,11 @@
       <c r="G22" s="22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="135" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="135" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="21" t="s">
         <v>37</v>
@@ -2397,8 +2696,12 @@
       <c r="G23" s="22" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="105" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="40">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21"/>
+    </row>
+    <row r="24" spans="1:9" ht="105" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="15" t="s">
         <v>3</v>
@@ -2418,8 +2721,11 @@
       <c r="G24" s="22" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="150" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="30" t="s">
         <v>40</v>
@@ -2439,8 +2745,12 @@
       <c r="G25" s="22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="105" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="40">
+        <v>1</v>
+      </c>
+      <c r="I25" s="21"/>
+    </row>
+    <row r="26" spans="1:9" ht="105" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="30" t="s">
         <v>41</v>
@@ -2460,8 +2770,11 @@
       <c r="G26" s="22" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="30" t="s">
         <v>42</v>
@@ -2481,8 +2794,12 @@
       <c r="G27" s="22" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="40">
+        <v>1</v>
+      </c>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -2491,9 +2808,14 @@
       <c r="D28" s="32"/>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" spans="1:7" ht="116.45" customHeight="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="32"/>
+      <c r="H28" s="42">
+        <f>AVERAGE(H29:H32)</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="1:9" ht="116.45" customHeight="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="15" t="s">
         <v>72</v>
@@ -2513,8 +2835,12 @@
       <c r="G29" s="34" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="116.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="40">
+        <v>1</v>
+      </c>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" ht="116.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="15" t="s">
         <v>44</v>
@@ -2534,8 +2860,11 @@
       <c r="G30" s="22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="15" t="s">
         <v>49</v>
@@ -2555,8 +2884,12 @@
       <c r="G31" s="22" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="40">
+        <v>1</v>
+      </c>
+      <c r="I31" s="21"/>
+    </row>
+    <row r="32" spans="1:9" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="15" t="s">
         <v>90</v>
@@ -2576,19 +2909,175 @@
       <c r="G32" s="22" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-    </row>
+      <c r="H32" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="46">
+        <f>(AVERAGE(H3:H11,H13:H15,H17:H27,H29:H32))</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="33"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="B3:G11 B13:G15 B17:G27 B29:G32">
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="28" priority="35">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="expression" dxfId="27" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="26" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="expression" dxfId="23" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:I9">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:I11">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2682,15 +3171,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100132AC456FB8E5746BFB1514B75DEDB26" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cab1b5aaea6c49ee10c7ddc906308699">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cdd62f4f-0f76-406d-bafb-c0159c105e45" xmlns:ns3="01098293-a8f5-4a21-8849-ffdc1d6b180f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd1255e5add0cffa97dc3ba80fadfc93" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2944,6 +3424,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2618A23-7192-4C37-970C-F0C1DE1142D7}">
   <ds:schemaRefs>
@@ -2963,14 +3452,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BD6E807-3B22-4452-A62C-6AF1CB49F76E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2325D13-BFF6-417E-8ACF-ABF97D6B5571}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2988,4 +3469,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BD6E807-3B22-4452-A62C-6AF1CB49F76E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>